<commit_message>
Properly handling start from1
</commit_message>
<xml_diff>
--- a/ExcelORM/ExcelORMTests/testFiles/columnsOnTheLeftHeaderNotFirstRow.xlsx
+++ b/ExcelORM/ExcelORMTests/testFiles/columnsOnTheLeftHeaderNotFirstRow.xlsx
@@ -1,17 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\piotr\Downloads\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42B9253F-6607-4886-A278-06AC5E9552F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="40" windowWidth="15960" windowHeight="18080"/>
+    <workbookView xWindow="83" yWindow="855" windowWidth="28717" windowHeight="14625" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet 1" sheetId="1" r:id="rId4"/>
+    <sheet name="Tab" sheetId="1" r:id="rId1"/>
+    <sheet name="WithTitle" sheetId="2" r:id="rId2"/>
   </sheets>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="15">
   <si>
     <t>First name</t>
   </si>
@@ -54,29 +64,19 @@
   <si>
     <t>Tester</t>
   </si>
+  <si>
+    <t>Big title</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="0" formatCode="General"/>
-  </numFmts>
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1">
     <font>
       <sz val="10"/>
       <color indexed="8"/>
       <name val="Helvetica Neue"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color indexed="8"/>
-      <name val="Helvetica Neue"/>
-    </font>
-    <font>
-      <sz val="15"/>
-      <color indexed="8"/>
-      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="3">
@@ -280,73 +280,76 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="21">
-    <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="15" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="12" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
+  <cellXfs count="22">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="15" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -356,26 +359,85 @@
   <tableStyles count="0"/>
   <colors>
     <indexedColors>
-      <rgbColor rgb="ff000000"/>
-      <rgbColor rgb="ffffffff"/>
-      <rgbColor rgb="ffff0000"/>
-      <rgbColor rgb="ff00ff00"/>
-      <rgbColor rgb="ff0000ff"/>
-      <rgbColor rgb="ffffff00"/>
-      <rgbColor rgb="ffff00ff"/>
-      <rgbColor rgb="ff00ffff"/>
-      <rgbColor rgb="ff000000"/>
-      <rgbColor rgb="ffffffff"/>
-      <rgbColor rgb="ffaaaaaa"/>
-      <rgbColor rgb="ffa5a5a5"/>
-      <rgbColor rgb="ff3f3f3f"/>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFAAAAAA"/>
+      <rgbColor rgb="FFA5A5A5"/>
+      <rgbColor rgb="FF3F3F3F"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Blank">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Blank">
   <a:themeElements>
     <a:clrScheme name="Blank">
       <a:dk1>
@@ -577,7 +639,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="50800" tIns="50800" rIns="50800" bIns="50800" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="50800" tIns="50800" rIns="50800" bIns="50800" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -595,7 +657,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1100" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -624,7 +686,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -649,7 +711,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -674,7 +736,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -699,7 +761,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -724,7 +786,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -749,7 +811,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -774,7 +836,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -799,7 +861,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -824,7 +886,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -837,9 +899,15 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:spDef>
@@ -856,7 +924,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
         <a:noAutofit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -874,7 +942,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -899,7 +967,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -924,7 +992,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -949,7 +1017,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -974,7 +1042,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -999,7 +1067,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1024,7 +1092,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1049,7 +1117,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1074,7 +1142,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1099,7 +1167,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1112,9 +1180,15 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:lnDef>
@@ -1128,7 +1202,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="50800" tIns="50800" rIns="50800" bIns="50800" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="50800" tIns="50800" rIns="50800" bIns="50800" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -1146,7 +1220,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1100" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1175,7 +1249,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1200,7 +1274,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1225,7 +1299,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1250,7 +1324,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1275,7 +1349,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1300,7 +1374,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1325,7 +1399,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1350,7 +1424,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1375,7 +1449,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1388,29 +1462,38 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:txDef>
   </a:objectDefaults>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F21"/>
   <sheetViews>
-    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="19.9" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="16.33203125" defaultRowHeight="19.899999999999999" customHeight="1"/>
   <cols>
-    <col min="1" max="6" width="16.3516" style="1" customWidth="1"/>
-    <col min="7" max="16384" width="16.3516" style="1" customWidth="1"/>
+    <col min="1" max="7" width="16.33203125" style="1" customWidth="1"/>
+    <col min="8" max="16384" width="16.33203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="20.25" customHeight="1">
+    <row r="1" spans="1:6" ht="20.25" customHeight="1">
       <c r="A1" s="2"/>
       <c r="B1" s="3"/>
       <c r="C1" s="4"/>
@@ -1418,7 +1501,7 @@
       <c r="E1" s="5"/>
       <c r="F1" s="5"/>
     </row>
-    <row r="2" ht="20.1" customHeight="1">
+    <row r="2" spans="1:6" ht="20.100000000000001" customHeight="1">
       <c r="A2" s="6"/>
       <c r="B2" s="7"/>
       <c r="C2" s="8"/>
@@ -1426,7 +1509,7 @@
       <c r="E2" s="9"/>
       <c r="F2" s="9"/>
     </row>
-    <row r="3" ht="20.1" customHeight="1">
+    <row r="3" spans="1:6" ht="20.100000000000001" customHeight="1">
       <c r="A3" s="6"/>
       <c r="B3" s="7"/>
       <c r="C3" s="8"/>
@@ -1434,7 +1517,7 @@
       <c r="E3" s="9"/>
       <c r="F3" s="9"/>
     </row>
-    <row r="4" ht="20.1" customHeight="1">
+    <row r="4" spans="1:6" ht="20.100000000000001" customHeight="1">
       <c r="A4" s="6"/>
       <c r="B4" s="7"/>
       <c r="C4" s="8"/>
@@ -1442,7 +1525,7 @@
       <c r="E4" s="9"/>
       <c r="F4" s="9"/>
     </row>
-    <row r="5" ht="20.1" customHeight="1">
+    <row r="5" spans="1:6" ht="20.100000000000001" customHeight="1">
       <c r="A5" s="10"/>
       <c r="B5" s="11"/>
       <c r="C5" s="12"/>
@@ -1450,7 +1533,7 @@
       <c r="E5" s="9"/>
       <c r="F5" s="9"/>
     </row>
-    <row r="6" ht="20.1" customHeight="1">
+    <row r="6" spans="1:6" ht="20.100000000000001" customHeight="1">
       <c r="A6" s="13"/>
       <c r="B6" s="9"/>
       <c r="C6" s="9"/>
@@ -1458,7 +1541,7 @@
       <c r="E6" s="9"/>
       <c r="F6" s="9"/>
     </row>
-    <row r="7" ht="20.1" customHeight="1">
+    <row r="7" spans="1:6" ht="20.100000000000001" customHeight="1">
       <c r="A7" s="13"/>
       <c r="B7" s="9"/>
       <c r="C7" s="14"/>
@@ -1466,77 +1549,77 @@
       <c r="E7" s="14"/>
       <c r="F7" s="9"/>
     </row>
-    <row r="8" ht="20.1" customHeight="1">
+    <row r="8" spans="1:6" ht="20.100000000000001" customHeight="1">
       <c r="A8" s="13"/>
       <c r="B8" s="15"/>
-      <c r="C8" t="s" s="16">
+      <c r="C8" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="D8" t="s" s="17">
+      <c r="D8" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="E8" t="s" s="17">
+      <c r="E8" s="17" t="s">
         <v>2</v>
       </c>
       <c r="F8" s="9"/>
     </row>
-    <row r="9" ht="20.1" customHeight="1">
+    <row r="9" spans="1:6" ht="20.100000000000001" customHeight="1">
       <c r="A9" s="13"/>
       <c r="B9" s="15"/>
-      <c r="C9" t="s" s="18">
+      <c r="C9" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="D9" t="s" s="19">
+      <c r="D9" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="E9" t="s" s="19">
+      <c r="E9" s="19" t="s">
         <v>5</v>
       </c>
       <c r="F9" s="9"/>
     </row>
-    <row r="10" ht="20.1" customHeight="1">
+    <row r="10" spans="1:6" ht="20.100000000000001" customHeight="1">
       <c r="A10" s="13"/>
       <c r="B10" s="15"/>
-      <c r="C10" t="s" s="18">
+      <c r="C10" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="D10" t="s" s="19">
+      <c r="D10" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="E10" t="s" s="19">
+      <c r="E10" s="19" t="s">
         <v>8</v>
       </c>
       <c r="F10" s="9"/>
     </row>
-    <row r="11" ht="20.1" customHeight="1">
+    <row r="11" spans="1:6" ht="20.100000000000001" customHeight="1">
       <c r="A11" s="13"/>
       <c r="B11" s="15"/>
-      <c r="C11" t="s" s="18">
+      <c r="C11" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="D11" t="s" s="19">
+      <c r="D11" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="E11" t="s" s="19">
+      <c r="E11" s="19" t="s">
         <v>11</v>
       </c>
       <c r="F11" s="9"/>
     </row>
-    <row r="12" ht="20.1" customHeight="1">
+    <row r="12" spans="1:6" ht="20.100000000000001" customHeight="1">
       <c r="A12" s="13"/>
       <c r="B12" s="15"/>
-      <c r="C12" t="s" s="18">
+      <c r="C12" s="18" t="s">
         <v>12</v>
       </c>
       <c r="D12" s="20">
         <v>3</v>
       </c>
-      <c r="E12" t="s" s="19">
+      <c r="E12" s="19" t="s">
         <v>13</v>
       </c>
       <c r="F12" s="9"/>
     </row>
-    <row r="13" ht="20.1" customHeight="1">
+    <row r="13" spans="1:6" ht="20.100000000000001" customHeight="1">
       <c r="A13" s="13"/>
       <c r="B13" s="9"/>
       <c r="C13" s="9"/>
@@ -1544,7 +1627,7 @@
       <c r="E13" s="9"/>
       <c r="F13" s="9"/>
     </row>
-    <row r="14" ht="20.1" customHeight="1">
+    <row r="14" spans="1:6" ht="20.100000000000001" customHeight="1">
       <c r="A14" s="13"/>
       <c r="B14" s="9"/>
       <c r="C14" s="9"/>
@@ -1552,7 +1635,7 @@
       <c r="E14" s="9"/>
       <c r="F14" s="9"/>
     </row>
-    <row r="15" ht="20.1" customHeight="1">
+    <row r="15" spans="1:6" ht="20.100000000000001" customHeight="1">
       <c r="A15" s="13"/>
       <c r="B15" s="9"/>
       <c r="C15" s="9"/>
@@ -1560,7 +1643,7 @@
       <c r="E15" s="9"/>
       <c r="F15" s="9"/>
     </row>
-    <row r="16" ht="20.1" customHeight="1">
+    <row r="16" spans="1:6" ht="20.100000000000001" customHeight="1">
       <c r="A16" s="13"/>
       <c r="B16" s="9"/>
       <c r="C16" s="9"/>
@@ -1568,7 +1651,7 @@
       <c r="E16" s="9"/>
       <c r="F16" s="9"/>
     </row>
-    <row r="17" ht="20.1" customHeight="1">
+    <row r="17" spans="1:6" ht="20.100000000000001" customHeight="1">
       <c r="A17" s="13"/>
       <c r="B17" s="9"/>
       <c r="C17" s="9"/>
@@ -1576,7 +1659,7 @@
       <c r="E17" s="9"/>
       <c r="F17" s="9"/>
     </row>
-    <row r="18" ht="20.1" customHeight="1">
+    <row r="18" spans="1:6" ht="20.100000000000001" customHeight="1">
       <c r="A18" s="13"/>
       <c r="B18" s="9"/>
       <c r="C18" s="9"/>
@@ -1584,7 +1667,7 @@
       <c r="E18" s="9"/>
       <c r="F18" s="9"/>
     </row>
-    <row r="19" ht="20.1" customHeight="1">
+    <row r="19" spans="1:6" ht="20.100000000000001" customHeight="1">
       <c r="A19" s="13"/>
       <c r="B19" s="9"/>
       <c r="C19" s="9"/>
@@ -1592,7 +1675,7 @@
       <c r="E19" s="9"/>
       <c r="F19" s="9"/>
     </row>
-    <row r="20" ht="20.1" customHeight="1">
+    <row r="20" spans="1:6" ht="20.100000000000001" customHeight="1">
       <c r="A20" s="13"/>
       <c r="B20" s="9"/>
       <c r="C20" s="9"/>
@@ -1600,7 +1683,7 @@
       <c r="E20" s="9"/>
       <c r="F20" s="9"/>
     </row>
-    <row r="21" ht="20.1" customHeight="1">
+    <row r="21" spans="1:6" ht="20.100000000000001" customHeight="1">
       <c r="A21" s="13"/>
       <c r="B21" s="9"/>
       <c r="C21" s="9"/>
@@ -1609,10 +1692,96 @@
       <c r="F21" s="9"/>
     </row>
   </sheetData>
-  <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.277778" footer="0.277778"/>
-  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="72" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
+  <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.27777800000000002" footer="0.27777800000000002"/>
+  <pageSetup scale="72" orientation="portrait"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED42C06A-1236-48DC-94CD-9A381361675F}">
+  <dimension ref="A1:I11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetData>
+    <row r="1" spans="1:9">
+      <c r="A1" s="21" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="21"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
+      <c r="F1" s="21"/>
+      <c r="G1" s="21"/>
+      <c r="H1" s="21"/>
+      <c r="I1" s="21"/>
+    </row>
+    <row r="7" spans="1:9" ht="25.5">
+      <c r="B7" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="C7" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="D7" s="17" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
+      <c r="B8" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="C8" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="D8" s="19" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="25.5">
+      <c r="B9" s="18" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="D9" s="19" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
+      <c r="B10" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="D10" s="19" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9">
+      <c r="B11" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="C11" s="20">
+        <v>3</v>
+      </c>
+      <c r="D11" s="19" t="s">
+        <v>13</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:I1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Checking for bad header
</commit_message>
<xml_diff>
--- a/ExcelORM/ExcelORMTests/testFiles/columnsOnTheLeftHeaderNotFirstRow.xlsx
+++ b/ExcelORM/ExcelORMTests/testFiles/columnsOnTheLeftHeaderNotFirstRow.xlsx
@@ -8,20 +8,21 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\piotr\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42B9253F-6607-4886-A278-06AC5E9552F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDAB312F-B540-496C-9AE0-5D06DE34E018}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="83" yWindow="855" windowWidth="28717" windowHeight="14625" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="83" yWindow="855" windowWidth="28717" windowHeight="14625" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tab" sheetId="1" r:id="rId1"/>
     <sheet name="WithTitle" sheetId="2" r:id="rId2"/>
+    <sheet name="BadHeader" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="17">
   <si>
     <t>First name</t>
   </si>
@@ -66,6 +67,12 @@
   </si>
   <si>
     <t>Big title</t>
+  </si>
+  <si>
+    <t>First</t>
+  </si>
+  <si>
+    <t>Last</t>
   </si>
 </sst>
 </file>
@@ -1484,7 +1491,7 @@
   <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.33203125" defaultRowHeight="19.899999999999999" customHeight="1"/>
@@ -1704,8 +1711,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED42C06A-1236-48DC-94CD-9A381361675F}">
   <dimension ref="A1:I11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B7" sqref="B7:D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -1784,4 +1791,74 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75A28E80-9A1E-428C-8E03-A7AB0384F56D}">
+  <dimension ref="A1:C5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetData>
+    <row r="1" spans="1:3" ht="25.5">
+      <c r="A1" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" s="17" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="19" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="25.5">
+      <c r="A3" s="18" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="19" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="19" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="20">
+        <v>3</v>
+      </c>
+      <c r="C5" s="19" t="s">
+        <v>13</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>